<commit_message>
update report and excel
</commit_message>
<xml_diff>
--- a/CV_template/import_cv_pseud.xlsx
+++ b/CV_template/import_cv_pseud.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cajordan\GIT\PowerBI\CV_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29AD7785-E591-4AB3-9D5A-2FA8015D2ADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B210FC32-F40D-4D71-BEBB-0A1BD4522D36}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D500CF17-8C35-4A90-9766-65F3CF7DAA40}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{D500CF17-8C35-4A90-9766-65F3CF7DAA40}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="798" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="833" uniqueCount="224">
   <si>
     <t>startdate</t>
   </si>
@@ -685,6 +685,36 @@
   </si>
   <si>
     <t>11.620579455237477</t>
+  </si>
+  <si>
+    <t>Webanalytics</t>
+  </si>
+  <si>
+    <t>Mobility / Tourism</t>
+  </si>
+  <si>
+    <t>Traffic Company</t>
+  </si>
+  <si>
+    <t>Data and Analytics Plattform: Webanalytics</t>
+  </si>
+  <si>
+    <t>Consultant / Power BI Developer</t>
+  </si>
+  <si>
+    <t>Implementation of a Power BI self-service solution</t>
+  </si>
+  <si>
+    <t>Design of data models</t>
+  </si>
+  <si>
+    <t>Development of datasets (Power Query M, DAX)</t>
+  </si>
+  <si>
+    <t>Conception and implementation of Power BI reports</t>
+  </si>
+  <si>
+    <t>Requirements gathering with business departments</t>
   </si>
 </sst>
 </file>
@@ -804,7 +834,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -821,63 +851,21 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="29">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor theme="4" tint="0.79998168889431442"/>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </top>
-        <bottom style="thin">
-          <color theme="4" tint="0.39997558519241921"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
     <dxf>
       <font>
         <b/>
@@ -991,6 +979,42 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="4" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -1521,8 +1545,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{40569263-420E-461A-8163-792F6349CFAB}" name="projects_table" displayName="projects_table" ref="A1:J24" totalsRowShown="0" headerRowDxfId="25">
-  <autoFilter ref="A1:J24" xr:uid="{40569263-420E-461A-8163-792F6349CFAB}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{40569263-420E-461A-8163-792F6349CFAB}" name="projects_table" displayName="projects_table" ref="A1:J31" totalsRowShown="0" headerRowDxfId="25">
+  <autoFilter ref="A1:J31" xr:uid="{40569263-420E-461A-8163-792F6349CFAB}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J24">
     <sortCondition descending="1" ref="A1:A24"/>
   </sortState>
@@ -1580,7 +1604,7 @@
     <tableColumn id="10" xr3:uid="{389774BB-2390-4593-8B14-BB9F71415424}" name="details"/>
     <tableColumn id="11" xr3:uid="{B9660891-3A23-4427-8EE6-6BD9DA2A4D66}" name="category" dataDxfId="8"/>
     <tableColumn id="12" xr3:uid="{460E435D-1343-455C-9EC6-FCB59809208D}" name="logo_url" dataDxfId="7"/>
-    <tableColumn id="13" xr3:uid="{0B2C2E59-4B81-4B94-B3B6-8FD9D9CB3E1E}" name="index_timeline" dataDxfId="0"/>
+    <tableColumn id="13" xr3:uid="{0B2C2E59-4B81-4B94-B3B6-8FD9D9CB3E1E}" name="index_timeline" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1590,18 +1614,18 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{E402CEBA-6B6B-4440-BFF4-B95D3362FD6D}" name="dim_location" displayName="dim_location" ref="A1:E9" totalsRowShown="0">
   <autoFilter ref="A1:E9" xr:uid="{E402CEBA-6B6B-4440-BFF4-B95D3362FD6D}"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B82AA2C3-0D9C-485D-B5E1-57043E54F1AB}" name="company_institution" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{DCC0837F-1E00-4FC0-9FEA-D1044399291B}" name="city" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{C6351892-F6A0-426A-B720-B65B67C40273}" name="country" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{85A84AAF-1CC4-48DA-B707-1292C18EB689}" name="longitute" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{A40284E0-B08A-4226-B35C-060027E792E7}" name="latitude" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{B82AA2C3-0D9C-485D-B5E1-57043E54F1AB}" name="company_institution" dataDxfId="5"/>
+    <tableColumn id="2" xr3:uid="{DCC0837F-1E00-4FC0-9FEA-D1044399291B}" name="city" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C6351892-F6A0-426A-B720-B65B67C40273}" name="country" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{85A84AAF-1CC4-48DA-B707-1292C18EB689}" name="longitute" dataDxfId="2"/>
+    <tableColumn id="5" xr3:uid="{A40284E0-B08A-4226-B35C-060027E792E7}" name="latitude" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A69D826A-8C3C-4A21-9BBD-CDD6B52D2B2F}" name="skills_tools_table" displayName="skills_tools_table" ref="A1:E35" totalsRowShown="0" headerRowDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{A69D826A-8C3C-4A21-9BBD-CDD6B52D2B2F}" name="skills_tools_table" displayName="skills_tools_table" ref="A1:E35" totalsRowShown="0" headerRowDxfId="0">
   <autoFilter ref="A1:E35" xr:uid="{A69D826A-8C3C-4A21-9BBD-CDD6B52D2B2F}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{89CA9609-E776-495B-A4F3-2C39074C0ABF}" name="category"/>
@@ -1913,7 +1937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7ACA714-72EC-4379-A169-0BAB6B81E9D6}">
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2030,21 +2054,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E63BE593-5581-44EE-B127-14A673C861AC}">
-  <dimension ref="A1:J24"/>
+  <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="11.5546875" style="1"/>
-    <col min="3" max="3" width="15.77734375" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
     <col min="4" max="4" width="26.21875" customWidth="1"/>
     <col min="5" max="5" width="11.109375" customWidth="1"/>
     <col min="6" max="6" width="12.77734375" customWidth="1"/>
     <col min="7" max="7" width="20.44140625" customWidth="1"/>
-    <col min="8" max="8" width="17.6640625" customWidth="1"/>
+    <col min="8" max="8" width="24.77734375" customWidth="1"/>
     <col min="9" max="9" width="30.109375" customWidth="1"/>
     <col min="10" max="10" width="79.88671875" customWidth="1"/>
   </cols>
@@ -2816,6 +2840,142 @@
       <c r="J24" t="s">
         <v>59</v>
       </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>45413</v>
+      </c>
+      <c r="C25" t="s">
+        <v>215</v>
+      </c>
+      <c r="D25" t="s">
+        <v>216</v>
+      </c>
+      <c r="E25" t="s">
+        <v>48</v>
+      </c>
+      <c r="G25" t="s">
+        <v>214</v>
+      </c>
+      <c r="H25" t="s">
+        <v>218</v>
+      </c>
+      <c r="I25" t="s">
+        <v>217</v>
+      </c>
+      <c r="J25" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>45414</v>
+      </c>
+      <c r="C26" t="s">
+        <v>215</v>
+      </c>
+      <c r="D26" t="s">
+        <v>216</v>
+      </c>
+      <c r="E26" t="s">
+        <v>48</v>
+      </c>
+      <c r="G26" t="s">
+        <v>214</v>
+      </c>
+      <c r="H26" t="s">
+        <v>218</v>
+      </c>
+      <c r="I26" t="s">
+        <v>217</v>
+      </c>
+      <c r="J26" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>45415</v>
+      </c>
+      <c r="C27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E27" t="s">
+        <v>48</v>
+      </c>
+      <c r="G27" t="s">
+        <v>214</v>
+      </c>
+      <c r="H27" t="s">
+        <v>218</v>
+      </c>
+      <c r="I27" t="s">
+        <v>217</v>
+      </c>
+      <c r="J27" s="22" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>45416</v>
+      </c>
+      <c r="C28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D28" t="s">
+        <v>216</v>
+      </c>
+      <c r="E28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G28" t="s">
+        <v>214</v>
+      </c>
+      <c r="H28" t="s">
+        <v>218</v>
+      </c>
+      <c r="I28" t="s">
+        <v>217</v>
+      </c>
+      <c r="J28" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>45417</v>
+      </c>
+      <c r="C29" t="s">
+        <v>215</v>
+      </c>
+      <c r="D29" t="s">
+        <v>216</v>
+      </c>
+      <c r="E29" t="s">
+        <v>48</v>
+      </c>
+      <c r="G29" t="s">
+        <v>214</v>
+      </c>
+      <c r="H29" t="s">
+        <v>218</v>
+      </c>
+      <c r="I29" t="s">
+        <v>217</v>
+      </c>
+      <c r="J29" s="22" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3654,10 +3814,10 @@
       <c r="A2" s="9">
         <v>42644</v>
       </c>
-      <c r="B2" s="19">
+      <c r="B2" s="17">
         <v>44012</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="18" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="3" t="s">
@@ -3685,7 +3845,7 @@
         <v>115</v>
       </c>
       <c r="L2" s="15"/>
-      <c r="M2" s="17">
+      <c r="M2" s="15">
         <v>1</v>
       </c>
     </row>
@@ -3693,10 +3853,10 @@
       <c r="A3" s="11">
         <v>42979</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="1">
         <v>43250</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" t="s">
         <v>9</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -3724,7 +3884,7 @@
         <v>115</v>
       </c>
       <c r="L3" s="3"/>
-      <c r="M3" s="16">
+      <c r="M3" s="3">
         <v>2</v>
       </c>
     </row>
@@ -3732,7 +3892,7 @@
       <c r="A4" s="9">
         <v>43647</v>
       </c>
-      <c r="B4" s="19">
+      <c r="B4" s="17">
         <v>43830</v>
       </c>
       <c r="C4" t="s">
@@ -3763,7 +3923,7 @@
         <v>114</v>
       </c>
       <c r="L4" s="3"/>
-      <c r="M4" s="16">
+      <c r="M4" s="3">
         <v>3</v>
       </c>
     </row>
@@ -3771,7 +3931,7 @@
       <c r="A5" s="11">
         <v>43647</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B5" s="1">
         <v>43830</v>
       </c>
       <c r="C5" t="s">
@@ -3802,7 +3962,7 @@
         <v>114</v>
       </c>
       <c r="L5" s="3"/>
-      <c r="M5" s="16">
+      <c r="M5" s="3">
         <v>3</v>
       </c>
     </row>
@@ -3810,7 +3970,7 @@
       <c r="A6" s="9">
         <v>43845</v>
       </c>
-      <c r="B6" s="19">
+      <c r="B6" s="17">
         <v>43905</v>
       </c>
       <c r="C6" t="s">
@@ -3841,7 +4001,7 @@
         <v>114</v>
       </c>
       <c r="L6" s="3"/>
-      <c r="M6" s="16">
+      <c r="M6" s="3">
         <v>4</v>
       </c>
     </row>
@@ -3849,7 +4009,7 @@
       <c r="A7" s="11">
         <v>43845</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B7" s="1">
         <v>43905</v>
       </c>
       <c r="C7" t="s">
@@ -3880,7 +4040,7 @@
         <v>114</v>
       </c>
       <c r="L7" s="3"/>
-      <c r="M7" s="16">
+      <c r="M7" s="3">
         <v>4</v>
       </c>
     </row>
@@ -3888,7 +4048,7 @@
       <c r="A8" s="9">
         <v>43845</v>
       </c>
-      <c r="B8" s="19">
+      <c r="B8" s="17">
         <v>43905</v>
       </c>
       <c r="C8" t="s">
@@ -3919,7 +4079,7 @@
         <v>114</v>
       </c>
       <c r="L8" s="3"/>
-      <c r="M8" s="16">
+      <c r="M8" s="3">
         <v>4</v>
       </c>
     </row>
@@ -3927,7 +4087,7 @@
       <c r="A9" s="11">
         <v>43845</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B9" s="1">
         <v>43905</v>
       </c>
       <c r="C9" t="s">
@@ -3958,7 +4118,7 @@
         <v>114</v>
       </c>
       <c r="L9" s="3"/>
-      <c r="M9" s="16">
+      <c r="M9" s="3">
         <v>4</v>
       </c>
     </row>
@@ -3969,7 +4129,7 @@
       <c r="B10" s="10">
         <v>45138</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D10" s="3" t="s">
@@ -3996,10 +4156,10 @@
       <c r="K10" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="L10" s="23" t="s">
+      <c r="L10" s="19" t="s">
         <v>134</v>
       </c>
-      <c r="M10" s="16">
+      <c r="M10" s="3">
         <v>5</v>
       </c>
     </row>
@@ -4038,7 +4198,7 @@
         <v>114</v>
       </c>
       <c r="L11" s="3"/>
-      <c r="M11" s="16">
+      <c r="M11" s="3">
         <v>6</v>
       </c>
     </row>
@@ -4077,7 +4237,7 @@
         <v>114</v>
       </c>
       <c r="L12" s="3"/>
-      <c r="M12" s="16">
+      <c r="M12" s="3">
         <v>6</v>
       </c>
     </row>
@@ -4116,7 +4276,7 @@
         <v>114</v>
       </c>
       <c r="L13" s="3"/>
-      <c r="M13" s="16">
+      <c r="M13" s="3">
         <v>6</v>
       </c>
     </row>
@@ -4155,7 +4315,7 @@
         <v>114</v>
       </c>
       <c r="L14" s="3"/>
-      <c r="M14" s="16">
+      <c r="M14" s="3">
         <v>6</v>
       </c>
     </row>
@@ -4193,7 +4353,7 @@
       <c r="K15" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="L15" s="16"/>
+      <c r="L15" s="3"/>
       <c r="M15" s="3">
         <v>7</v>
       </c>
@@ -4232,7 +4392,7 @@
       <c r="K16" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="L16" s="16"/>
+      <c r="L16" s="3"/>
       <c r="M16" s="3">
         <v>7</v>
       </c>
@@ -4271,7 +4431,7 @@
       <c r="K17" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="L17" s="16"/>
+      <c r="L17" s="3"/>
       <c r="M17" s="3">
         <v>7</v>
       </c>
@@ -4310,7 +4470,7 @@
       <c r="K18" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="L18" s="16"/>
+      <c r="L18" s="3"/>
       <c r="M18" s="3">
         <v>7</v>
       </c>
@@ -4350,7 +4510,7 @@
         <v>113</v>
       </c>
       <c r="L19" s="3"/>
-      <c r="M19" s="16">
+      <c r="M19" s="3">
         <v>8</v>
       </c>
     </row>
@@ -4389,7 +4549,7 @@
         <v>113</v>
       </c>
       <c r="L20" s="3"/>
-      <c r="M20" s="16">
+      <c r="M20" s="3">
         <v>8</v>
       </c>
     </row>
@@ -4428,7 +4588,7 @@
         <v>113</v>
       </c>
       <c r="L21" s="3"/>
-      <c r="M21" s="16">
+      <c r="M21" s="3">
         <v>8</v>
       </c>
     </row>
@@ -4467,7 +4627,7 @@
         <v>113</v>
       </c>
       <c r="L22" s="3"/>
-      <c r="M22" s="16">
+      <c r="M22" s="3">
         <v>8</v>
       </c>
     </row>
@@ -4506,7 +4666,7 @@
         <v>113</v>
       </c>
       <c r="L23" s="3"/>
-      <c r="M23" s="16">
+      <c r="M23" s="3">
         <v>8</v>
       </c>
     </row>
@@ -4520,7 +4680,7 @@
       <c r="C24" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" t="s">
         <v>94</v>
       </c>
       <c r="E24" s="4" t="s">
@@ -4545,7 +4705,7 @@
         <v>113</v>
       </c>
       <c r="L24" s="3"/>
-      <c r="M24" s="16">
+      <c r="M24" s="3">
         <v>8</v>
       </c>
     </row>
@@ -4559,7 +4719,7 @@
       <c r="C25" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="18" t="s">
         <v>94</v>
       </c>
       <c r="E25" s="3" t="s">
@@ -4584,7 +4744,7 @@
         <v>113</v>
       </c>
       <c r="L25" s="3"/>
-      <c r="M25" s="16">
+      <c r="M25" s="3">
         <v>8</v>
       </c>
     </row>
@@ -4598,7 +4758,7 @@
       <c r="C26" s="4" t="s">
         <v>201</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" t="s">
         <v>94</v>
       </c>
       <c r="E26" s="4" t="s">
@@ -4622,20 +4782,20 @@
       <c r="K26" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L26" s="24"/>
-      <c r="M26" s="18">
+      <c r="L26" s="16"/>
+      <c r="M26" s="16">
         <v>8</v>
       </c>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="25">
+      <c r="A27" s="9">
         <v>45413</v>
       </c>
-      <c r="B27" s="26"/>
-      <c r="C27" s="16" t="s">
+      <c r="B27" s="10"/>
+      <c r="C27" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D27" s="27" t="s">
+      <c r="D27" s="18" t="s">
         <v>210</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -4647,10 +4807,10 @@
       <c r="G27" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H27" s="16" t="s">
+      <c r="H27" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="I27" s="16" t="s">
+      <c r="I27" s="3" t="s">
         <v>209</v>
       </c>
       <c r="J27" t="s">
@@ -4659,18 +4819,18 @@
       <c r="K27" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L27" s="16"/>
-      <c r="M27" s="16"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="25">
+      <c r="A28" s="9">
         <v>45413</v>
       </c>
-      <c r="B28" s="26"/>
-      <c r="C28" s="16" t="s">
+      <c r="B28" s="10"/>
+      <c r="C28" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D28" s="27" t="s">
+      <c r="D28" s="18" t="s">
         <v>210</v>
       </c>
       <c r="E28" s="4" t="s">
@@ -4682,10 +4842,10 @@
       <c r="G28" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H28" s="16" t="s">
+      <c r="H28" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="I28" s="16" t="s">
+      <c r="I28" s="3" t="s">
         <v>209</v>
       </c>
       <c r="J28" t="s">
@@ -4694,18 +4854,18 @@
       <c r="K28" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L28" s="16"/>
-      <c r="M28" s="16"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="25">
+      <c r="A29" s="9">
         <v>45413</v>
       </c>
-      <c r="B29" s="28"/>
-      <c r="C29" s="16" t="s">
+      <c r="B29" s="20"/>
+      <c r="C29" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="18" t="s">
         <v>210</v>
       </c>
       <c r="E29" s="4" t="s">
@@ -4717,20 +4877,20 @@
       <c r="G29" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="H29" s="16" t="s">
+      <c r="H29" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="I29" s="16" t="s">
+      <c r="I29" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="J29" s="22" t="s">
+      <c r="J29" t="s">
         <v>14</v>
       </c>
       <c r="K29" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="L29" s="18"/>
-      <c r="M29" s="18"/>
+      <c r="L29" s="16"/>
+      <c r="M29" s="16"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -4895,7 +5055,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="21" t="s">
         <v>211</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -4904,10 +5064,10 @@
       <c r="C9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="2" t="s">
         <v>212</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="2" t="s">
         <v>213</v>
       </c>
     </row>

</xml_diff>